<commit_message>
Solo falta length, type y offset
</commit_message>
<xml_diff>
--- a/1toolConverter_local/backend/Cefa/cefa.xlsx
+++ b/1toolConverter_local/backend/Cefa/cefa.xlsx
@@ -651,7 +651,7 @@
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S2" t="inlineStr"/>
@@ -755,7 +755,7 @@
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S3" t="inlineStr"/>
@@ -859,7 +859,7 @@
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S4" t="inlineStr"/>
@@ -963,7 +963,7 @@
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S5" t="inlineStr"/>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S6" t="inlineStr"/>
@@ -1171,7 +1171,7 @@
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S7" t="inlineStr"/>
@@ -1275,7 +1275,7 @@
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S8" t="inlineStr"/>
@@ -1379,7 +1379,7 @@
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S9" t="inlineStr"/>
@@ -1483,7 +1483,7 @@
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S10" t="inlineStr"/>
@@ -1587,7 +1587,7 @@
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S11" t="inlineStr"/>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S12" t="inlineStr"/>
@@ -1795,7 +1795,7 @@
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S13" t="inlineStr"/>
@@ -1899,7 +1899,7 @@
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S14" t="inlineStr"/>
@@ -2003,7 +2003,7 @@
       </c>
       <c r="R15" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S15" t="inlineStr"/>
@@ -2107,7 +2107,7 @@
       </c>
       <c r="R16" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S16" t="inlineStr"/>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="R17" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S17" t="inlineStr"/>
@@ -2315,7 +2315,7 @@
       </c>
       <c r="R18" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S18" t="inlineStr"/>
@@ -2419,7 +2419,7 @@
       </c>
       <c r="R19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S19" t="inlineStr"/>
@@ -2523,7 +2523,7 @@
       </c>
       <c r="R20" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S20" t="inlineStr"/>
@@ -2627,7 +2627,7 @@
       </c>
       <c r="R21" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S21" t="inlineStr"/>
@@ -2731,7 +2731,7 @@
       </c>
       <c r="R22" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S22" t="inlineStr"/>
@@ -2835,7 +2835,7 @@
       </c>
       <c r="R23" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S23" t="inlineStr"/>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="R24" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S24" t="inlineStr"/>
@@ -3043,7 +3043,7 @@
       </c>
       <c r="R25" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S25" t="inlineStr"/>
@@ -3147,7 +3147,7 @@
       </c>
       <c r="R26" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S26" t="inlineStr"/>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="R27" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S27" t="inlineStr"/>
@@ -3355,7 +3355,7 @@
       </c>
       <c r="R28" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S28" t="inlineStr"/>
@@ -3459,7 +3459,7 @@
       </c>
       <c r="R29" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S29" t="inlineStr"/>
@@ -3563,7 +3563,7 @@
       </c>
       <c r="R30" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S30" t="inlineStr"/>
@@ -3667,7 +3667,7 @@
       </c>
       <c r="R31" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S31" t="inlineStr"/>
@@ -3771,7 +3771,7 @@
       </c>
       <c r="R32" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S32" t="inlineStr"/>
@@ -3875,7 +3875,7 @@
       </c>
       <c r="R33" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S33" t="inlineStr"/>
@@ -3979,7 +3979,7 @@
       </c>
       <c r="R34" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S34" t="inlineStr"/>
@@ -4083,7 +4083,7 @@
       </c>
       <c r="R35" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S35" t="inlineStr"/>
@@ -4187,7 +4187,7 @@
       </c>
       <c r="R36" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S36" t="inlineStr"/>
@@ -4291,7 +4291,7 @@
       </c>
       <c r="R37" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S37" t="inlineStr"/>
@@ -4395,7 +4395,7 @@
       </c>
       <c r="R38" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S38" t="inlineStr"/>
@@ -4499,7 +4499,7 @@
       </c>
       <c r="R39" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S39" t="inlineStr"/>
@@ -4603,7 +4603,7 @@
       </c>
       <c r="R40" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S40" t="inlineStr"/>
@@ -4707,7 +4707,7 @@
       </c>
       <c r="R41" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S41" t="inlineStr"/>
@@ -4811,7 +4811,7 @@
       </c>
       <c r="R42" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S42" t="inlineStr"/>
@@ -4884,7 +4884,7 @@
         </is>
       </c>
       <c r="H43" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I43" t="n">
         <v>1</v>
@@ -4915,7 +4915,7 @@
       </c>
       <c r="R43" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S43" t="inlineStr"/>
@@ -4988,7 +4988,7 @@
         </is>
       </c>
       <c r="H44" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I44" t="n">
         <v>1</v>
@@ -5019,7 +5019,7 @@
       </c>
       <c r="R44" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S44" t="inlineStr"/>
@@ -5092,7 +5092,7 @@
         </is>
       </c>
       <c r="H45" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I45" t="n">
         <v>1</v>
@@ -5123,7 +5123,7 @@
       </c>
       <c r="R45" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S45" t="inlineStr"/>
@@ -5196,7 +5196,7 @@
         </is>
       </c>
       <c r="H46" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I46" t="n">
         <v>1</v>
@@ -5227,7 +5227,7 @@
       </c>
       <c r="R46" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S46" t="inlineStr"/>
@@ -5300,7 +5300,7 @@
         </is>
       </c>
       <c r="H47" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I47" t="n">
         <v>1</v>
@@ -5331,7 +5331,7 @@
       </c>
       <c r="R47" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S47" t="inlineStr"/>
@@ -5404,7 +5404,7 @@
         </is>
       </c>
       <c r="H48" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I48" t="n">
         <v>1</v>
@@ -5435,7 +5435,7 @@
       </c>
       <c r="R48" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S48" t="inlineStr"/>
@@ -5508,7 +5508,7 @@
         </is>
       </c>
       <c r="H49" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I49" t="n">
         <v>1</v>
@@ -5539,7 +5539,7 @@
       </c>
       <c r="R49" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S49" t="inlineStr"/>
@@ -5612,7 +5612,7 @@
         </is>
       </c>
       <c r="H50" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I50" t="n">
         <v>1</v>
@@ -5643,7 +5643,7 @@
       </c>
       <c r="R50" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S50" t="inlineStr"/>
@@ -5716,7 +5716,7 @@
         </is>
       </c>
       <c r="H51" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I51" t="n">
         <v>1</v>
@@ -5747,7 +5747,7 @@
       </c>
       <c r="R51" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S51" t="inlineStr"/>
@@ -5820,7 +5820,7 @@
         </is>
       </c>
       <c r="H52" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I52" t="n">
         <v>1</v>
@@ -5851,7 +5851,7 @@
       </c>
       <c r="R52" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S52" t="inlineStr"/>
@@ -5924,7 +5924,7 @@
         </is>
       </c>
       <c r="H53" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I53" t="n">
         <v>1</v>
@@ -5955,7 +5955,7 @@
       </c>
       <c r="R53" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S53" t="inlineStr"/>
@@ -6028,7 +6028,7 @@
         </is>
       </c>
       <c r="H54" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I54" t="n">
         <v>1</v>
@@ -6059,7 +6059,7 @@
       </c>
       <c r="R54" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S54" t="inlineStr"/>
@@ -6132,7 +6132,7 @@
         </is>
       </c>
       <c r="H55" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I55" t="n">
         <v>1</v>
@@ -6163,7 +6163,7 @@
       </c>
       <c r="R55" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S55" t="inlineStr"/>
@@ -6236,7 +6236,7 @@
         </is>
       </c>
       <c r="H56" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I56" t="n">
         <v>1</v>
@@ -6267,7 +6267,7 @@
       </c>
       <c r="R56" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S56" t="inlineStr"/>
@@ -6340,7 +6340,7 @@
         </is>
       </c>
       <c r="H57" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I57" t="n">
         <v>1</v>
@@ -6371,7 +6371,7 @@
       </c>
       <c r="R57" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S57" t="inlineStr"/>
@@ -6444,7 +6444,7 @@
         </is>
       </c>
       <c r="H58" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I58" t="n">
         <v>1</v>
@@ -6475,7 +6475,7 @@
       </c>
       <c r="R58" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S58" t="inlineStr"/>
@@ -6548,7 +6548,7 @@
         </is>
       </c>
       <c r="H59" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I59" t="n">
         <v>1</v>
@@ -6579,7 +6579,7 @@
       </c>
       <c r="R59" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S59" t="inlineStr"/>
@@ -6652,7 +6652,7 @@
         </is>
       </c>
       <c r="H60" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I60" t="n">
         <v>1</v>
@@ -6683,7 +6683,7 @@
       </c>
       <c r="R60" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S60" t="inlineStr"/>
@@ -6756,7 +6756,7 @@
         </is>
       </c>
       <c r="H61" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I61" t="n">
         <v>1</v>
@@ -6787,7 +6787,7 @@
       </c>
       <c r="R61" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S61" t="inlineStr"/>
@@ -6860,7 +6860,7 @@
         </is>
       </c>
       <c r="H62" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I62" t="n">
         <v>1</v>
@@ -6891,7 +6891,7 @@
       </c>
       <c r="R62" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S62" t="inlineStr"/>
@@ -6964,7 +6964,7 @@
         </is>
       </c>
       <c r="H63" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I63" t="n">
         <v>1</v>
@@ -6995,7 +6995,7 @@
       </c>
       <c r="R63" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S63" t="inlineStr"/>
@@ -7068,7 +7068,7 @@
         </is>
       </c>
       <c r="H64" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I64" t="n">
         <v>1</v>
@@ -7099,7 +7099,7 @@
       </c>
       <c r="R64" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S64" t="inlineStr"/>
@@ -7172,7 +7172,7 @@
         </is>
       </c>
       <c r="H65" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I65" t="n">
         <v>1</v>
@@ -7203,7 +7203,7 @@
       </c>
       <c r="R65" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S65" t="inlineStr"/>
@@ -7276,7 +7276,7 @@
         </is>
       </c>
       <c r="H66" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I66" t="n">
         <v>1</v>
@@ -7307,7 +7307,7 @@
       </c>
       <c r="R66" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S66" t="inlineStr"/>
@@ -7380,7 +7380,7 @@
         </is>
       </c>
       <c r="H67" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I67" t="n">
         <v>1</v>
@@ -7411,7 +7411,7 @@
       </c>
       <c r="R67" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S67" t="inlineStr"/>
@@ -7484,7 +7484,7 @@
         </is>
       </c>
       <c r="H68" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I68" t="n">
         <v>1</v>
@@ -7515,7 +7515,7 @@
       </c>
       <c r="R68" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S68" t="inlineStr"/>
@@ -7588,7 +7588,7 @@
         </is>
       </c>
       <c r="H69" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I69" t="n">
         <v>1</v>
@@ -7619,7 +7619,7 @@
       </c>
       <c r="R69" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S69" t="inlineStr"/>
@@ -7692,7 +7692,7 @@
         </is>
       </c>
       <c r="H70" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I70" t="n">
         <v>1</v>
@@ -7723,7 +7723,7 @@
       </c>
       <c r="R70" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S70" t="inlineStr"/>
@@ -7796,7 +7796,7 @@
         </is>
       </c>
       <c r="H71" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I71" t="n">
         <v>1</v>
@@ -7827,7 +7827,7 @@
       </c>
       <c r="R71" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S71" t="inlineStr"/>
@@ -7900,7 +7900,7 @@
         </is>
       </c>
       <c r="H72" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I72" t="n">
         <v>1</v>
@@ -7931,7 +7931,7 @@
       </c>
       <c r="R72" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S72" t="inlineStr"/>
@@ -8004,7 +8004,7 @@
         </is>
       </c>
       <c r="H73" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I73" t="n">
         <v>1</v>
@@ -8035,7 +8035,7 @@
       </c>
       <c r="R73" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S73" t="inlineStr"/>
@@ -8108,7 +8108,7 @@
         </is>
       </c>
       <c r="H74" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I74" t="n">
         <v>3</v>
@@ -8143,7 +8143,7 @@
       </c>
       <c r="R74" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>s16</t>
         </is>
       </c>
       <c r="S74" t="inlineStr"/>
@@ -8216,7 +8216,7 @@
         </is>
       </c>
       <c r="H75" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I75" t="n">
         <v>3</v>
@@ -8251,7 +8251,7 @@
       </c>
       <c r="R75" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>s16</t>
         </is>
       </c>
       <c r="S75" t="inlineStr"/>
@@ -8324,7 +8324,7 @@
         </is>
       </c>
       <c r="H76" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I76" t="n">
         <v>3</v>
@@ -8359,7 +8359,7 @@
       </c>
       <c r="R76" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>s16</t>
         </is>
       </c>
       <c r="S76" t="inlineStr"/>
@@ -8432,7 +8432,7 @@
         </is>
       </c>
       <c r="H77" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I77" t="n">
         <v>3</v>
@@ -8467,7 +8467,7 @@
       </c>
       <c r="R77" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>s16</t>
         </is>
       </c>
       <c r="S77" t="inlineStr"/>
@@ -8540,7 +8540,7 @@
         </is>
       </c>
       <c r="H78" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I78" t="n">
         <v>3</v>
@@ -8575,7 +8575,7 @@
       </c>
       <c r="R78" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>s16</t>
         </is>
       </c>
       <c r="S78" t="inlineStr"/>
@@ -8648,7 +8648,7 @@
         </is>
       </c>
       <c r="H79" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I79" t="n">
         <v>3</v>
@@ -8683,7 +8683,7 @@
       </c>
       <c r="R79" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>s16</t>
         </is>
       </c>
       <c r="S79" t="inlineStr"/>
@@ -8756,7 +8756,7 @@
         </is>
       </c>
       <c r="H80" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I80" t="n">
         <v>3</v>
@@ -8791,7 +8791,7 @@
       </c>
       <c r="R80" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>s16</t>
         </is>
       </c>
       <c r="S80" t="inlineStr"/>
@@ -8864,7 +8864,7 @@
         </is>
       </c>
       <c r="H81" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I81" t="n">
         <v>3</v>
@@ -8899,7 +8899,7 @@
       </c>
       <c r="R81" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>s16</t>
         </is>
       </c>
       <c r="S81" t="inlineStr"/>
@@ -8972,7 +8972,7 @@
         </is>
       </c>
       <c r="H82" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I82" t="n">
         <v>3</v>
@@ -9007,7 +9007,7 @@
       </c>
       <c r="R82" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>s16</t>
         </is>
       </c>
       <c r="S82" t="inlineStr"/>
@@ -9080,7 +9080,7 @@
         </is>
       </c>
       <c r="H83" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I83" t="n">
         <v>3</v>
@@ -9115,7 +9115,7 @@
       </c>
       <c r="R83" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>s16</t>
         </is>
       </c>
       <c r="S83" t="inlineStr"/>
@@ -9188,7 +9188,7 @@
         </is>
       </c>
       <c r="H84" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I84" t="n">
         <v>3</v>
@@ -9223,7 +9223,7 @@
       </c>
       <c r="R84" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>s16</t>
         </is>
       </c>
       <c r="S84" t="inlineStr"/>
@@ -9296,7 +9296,7 @@
         </is>
       </c>
       <c r="H85" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I85" t="n">
         <v>3</v>
@@ -9331,7 +9331,7 @@
       </c>
       <c r="R85" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>s16</t>
         </is>
       </c>
       <c r="S85" t="inlineStr"/>
@@ -9404,7 +9404,7 @@
         </is>
       </c>
       <c r="H86" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I86" t="n">
         <v>3</v>
@@ -9439,7 +9439,7 @@
       </c>
       <c r="R86" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>s16</t>
         </is>
       </c>
       <c r="S86" t="inlineStr"/>
@@ -9512,7 +9512,7 @@
         </is>
       </c>
       <c r="H87" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I87" t="n">
         <v>3</v>
@@ -9547,7 +9547,7 @@
       </c>
       <c r="R87" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>s16</t>
         </is>
       </c>
       <c r="S87" t="inlineStr"/>
@@ -9620,7 +9620,7 @@
         </is>
       </c>
       <c r="H88" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I88" t="n">
         <v>3</v>
@@ -9655,7 +9655,7 @@
       </c>
       <c r="R88" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>s16</t>
         </is>
       </c>
       <c r="S88" t="inlineStr"/>
@@ -9728,7 +9728,7 @@
         </is>
       </c>
       <c r="H89" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I89" t="n">
         <v>3</v>
@@ -9763,7 +9763,7 @@
       </c>
       <c r="R89" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>s16</t>
         </is>
       </c>
       <c r="S89" t="inlineStr"/>
@@ -9836,7 +9836,7 @@
         </is>
       </c>
       <c r="H90" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I90" t="n">
         <v>3</v>
@@ -9871,7 +9871,7 @@
       </c>
       <c r="R90" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>s16</t>
         </is>
       </c>
       <c r="S90" t="inlineStr"/>
@@ -9944,7 +9944,7 @@
         </is>
       </c>
       <c r="H91" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I91" t="n">
         <v>3</v>
@@ -9979,7 +9979,7 @@
       </c>
       <c r="R91" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>s16</t>
         </is>
       </c>
       <c r="S91" t="inlineStr"/>
@@ -10052,7 +10052,7 @@
         </is>
       </c>
       <c r="H92" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I92" t="n">
         <v>3</v>
@@ -10087,7 +10087,7 @@
       </c>
       <c r="R92" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>s16</t>
         </is>
       </c>
       <c r="S92" t="inlineStr"/>
@@ -10160,7 +10160,7 @@
         </is>
       </c>
       <c r="H93" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I93" t="n">
         <v>3</v>
@@ -10195,7 +10195,7 @@
       </c>
       <c r="R93" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>s16</t>
         </is>
       </c>
       <c r="S93" t="inlineStr"/>
@@ -10268,7 +10268,7 @@
         </is>
       </c>
       <c r="H94" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I94" t="n">
         <v>3</v>
@@ -10303,7 +10303,7 @@
       </c>
       <c r="R94" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>s16</t>
         </is>
       </c>
       <c r="S94" t="inlineStr"/>
@@ -10376,7 +10376,7 @@
         </is>
       </c>
       <c r="H95" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I95" t="n">
         <v>3</v>
@@ -10411,7 +10411,7 @@
       </c>
       <c r="R95" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>s16</t>
         </is>
       </c>
       <c r="S95" t="inlineStr"/>
@@ -10484,7 +10484,7 @@
         </is>
       </c>
       <c r="H96" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I96" t="n">
         <v>3</v>
@@ -10519,7 +10519,7 @@
       </c>
       <c r="R96" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>s16</t>
         </is>
       </c>
       <c r="S96" t="inlineStr"/>
@@ -10592,7 +10592,7 @@
         </is>
       </c>
       <c r="H97" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I97" t="n">
         <v>3</v>
@@ -10627,7 +10627,7 @@
       </c>
       <c r="R97" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>s16</t>
         </is>
       </c>
       <c r="S97" t="inlineStr"/>
@@ -10700,7 +10700,7 @@
         </is>
       </c>
       <c r="H98" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I98" t="n">
         <v>3</v>
@@ -10735,7 +10735,7 @@
       </c>
       <c r="R98" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>s16</t>
         </is>
       </c>
       <c r="S98" t="inlineStr"/>
@@ -10808,7 +10808,7 @@
         </is>
       </c>
       <c r="H99" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I99" t="n">
         <v>3</v>
@@ -10843,7 +10843,7 @@
       </c>
       <c r="R99" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>s16</t>
         </is>
       </c>
       <c r="S99" t="inlineStr"/>
@@ -10916,7 +10916,7 @@
         </is>
       </c>
       <c r="H100" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I100" t="n">
         <v>3</v>
@@ -10951,7 +10951,7 @@
       </c>
       <c r="R100" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>s16</t>
         </is>
       </c>
       <c r="S100" t="inlineStr"/>
@@ -11024,7 +11024,7 @@
         </is>
       </c>
       <c r="H101" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I101" t="n">
         <v>3</v>
@@ -11059,7 +11059,7 @@
       </c>
       <c r="R101" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>s16</t>
         </is>
       </c>
       <c r="S101" t="inlineStr"/>
@@ -11132,7 +11132,7 @@
         </is>
       </c>
       <c r="H102" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I102" t="n">
         <v>3</v>
@@ -11167,7 +11167,7 @@
       </c>
       <c r="R102" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>s16</t>
         </is>
       </c>
       <c r="S102" t="inlineStr"/>
@@ -11240,7 +11240,7 @@
         </is>
       </c>
       <c r="H103" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I103" t="n">
         <v>3</v>
@@ -11275,7 +11275,7 @@
       </c>
       <c r="R103" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>s16</t>
         </is>
       </c>
       <c r="S103" t="inlineStr"/>
@@ -11348,7 +11348,7 @@
         </is>
       </c>
       <c r="H104" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I104" t="n">
         <v>3</v>
@@ -11383,7 +11383,7 @@
       </c>
       <c r="R104" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>s16</t>
         </is>
       </c>
       <c r="S104" t="inlineStr"/>
@@ -11456,7 +11456,7 @@
         </is>
       </c>
       <c r="H105" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I105" t="n">
         <v>3</v>
@@ -11491,7 +11491,7 @@
       </c>
       <c r="R105" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>s16</t>
         </is>
       </c>
       <c r="S105" t="inlineStr"/>
@@ -11564,7 +11564,7 @@
         </is>
       </c>
       <c r="H106" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I106" t="n">
         <v>3</v>
@@ -11599,7 +11599,7 @@
       </c>
       <c r="R106" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>s16</t>
         </is>
       </c>
       <c r="S106" t="inlineStr"/>
@@ -11672,7 +11672,7 @@
         </is>
       </c>
       <c r="H107" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I107" t="n">
         <v>3</v>
@@ -11707,7 +11707,7 @@
       </c>
       <c r="R107" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>s16</t>
         </is>
       </c>
       <c r="S107" t="inlineStr"/>
@@ -11780,7 +11780,7 @@
         </is>
       </c>
       <c r="H108" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I108" t="n">
         <v>3</v>
@@ -11815,7 +11815,7 @@
       </c>
       <c r="R108" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>s16</t>
         </is>
       </c>
       <c r="S108" t="inlineStr"/>
@@ -11888,7 +11888,7 @@
         </is>
       </c>
       <c r="H109" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I109" t="n">
         <v>3</v>
@@ -11923,7 +11923,7 @@
       </c>
       <c r="R109" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>s16</t>
         </is>
       </c>
       <c r="S109" t="inlineStr"/>
@@ -11996,7 +11996,7 @@
         </is>
       </c>
       <c r="H110" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I110" t="n">
         <v>3</v>
@@ -12031,7 +12031,7 @@
       </c>
       <c r="R110" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>s16</t>
         </is>
       </c>
       <c r="S110" t="inlineStr"/>
@@ -12104,7 +12104,7 @@
         </is>
       </c>
       <c r="H111" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I111" t="n">
         <v>3</v>
@@ -12139,7 +12139,7 @@
       </c>
       <c r="R111" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>s16</t>
         </is>
       </c>
       <c r="S111" t="inlineStr"/>
@@ -12212,7 +12212,7 @@
         </is>
       </c>
       <c r="H112" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I112" t="n">
         <v>3</v>
@@ -12247,7 +12247,7 @@
       </c>
       <c r="R112" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>s16</t>
         </is>
       </c>
       <c r="S112" t="inlineStr"/>
@@ -12351,7 +12351,7 @@
       </c>
       <c r="R113" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S113" t="inlineStr"/>
@@ -12455,7 +12455,7 @@
       </c>
       <c r="R114" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S114" t="inlineStr"/>
@@ -12559,7 +12559,7 @@
       </c>
       <c r="R115" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S115" t="inlineStr"/>
@@ -12663,7 +12663,7 @@
       </c>
       <c r="R116" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S116" t="inlineStr"/>
@@ -12767,7 +12767,7 @@
       </c>
       <c r="R117" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S117" t="inlineStr"/>
@@ -12871,7 +12871,7 @@
       </c>
       <c r="R118" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S118" t="inlineStr"/>
@@ -12975,7 +12975,7 @@
       </c>
       <c r="R119" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S119" t="inlineStr"/>
@@ -13079,7 +13079,7 @@
       </c>
       <c r="R120" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S120" t="inlineStr"/>
@@ -13183,7 +13183,7 @@
       </c>
       <c r="R121" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S121" t="inlineStr"/>
@@ -13287,7 +13287,7 @@
       </c>
       <c r="R122" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S122" t="inlineStr"/>
@@ -13391,7 +13391,7 @@
       </c>
       <c r="R123" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S123" t="inlineStr"/>
@@ -13495,7 +13495,7 @@
       </c>
       <c r="R124" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S124" t="inlineStr"/>
@@ -13599,7 +13599,7 @@
       </c>
       <c r="R125" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S125" t="inlineStr"/>
@@ -13703,7 +13703,7 @@
       </c>
       <c r="R126" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S126" t="inlineStr"/>
@@ -13807,7 +13807,7 @@
       </c>
       <c r="R127" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S127" t="inlineStr"/>
@@ -13911,7 +13911,7 @@
       </c>
       <c r="R128" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S128" t="inlineStr"/>
@@ -14015,7 +14015,7 @@
       </c>
       <c r="R129" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S129" t="inlineStr"/>
@@ -14119,7 +14119,7 @@
       </c>
       <c r="R130" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S130" t="inlineStr"/>
@@ -14223,7 +14223,7 @@
       </c>
       <c r="R131" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S131" t="inlineStr"/>
@@ -14327,7 +14327,7 @@
       </c>
       <c r="R132" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S132" t="inlineStr"/>
@@ -14431,7 +14431,7 @@
       </c>
       <c r="R133" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S133" t="inlineStr"/>
@@ -14535,7 +14535,7 @@
       </c>
       <c r="R134" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S134" t="inlineStr"/>
@@ -14639,7 +14639,7 @@
       </c>
       <c r="R135" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S135" t="inlineStr"/>
@@ -14743,7 +14743,7 @@
       </c>
       <c r="R136" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S136" t="inlineStr"/>
@@ -14847,7 +14847,7 @@
       </c>
       <c r="R137" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S137" t="inlineStr"/>
@@ -14951,7 +14951,7 @@
       </c>
       <c r="R138" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S138" t="inlineStr"/>
@@ -15055,7 +15055,7 @@
       </c>
       <c r="R139" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S139" t="inlineStr"/>
@@ -15159,7 +15159,7 @@
       </c>
       <c r="R140" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S140" t="inlineStr"/>
@@ -15263,7 +15263,7 @@
       </c>
       <c r="R141" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S141" t="inlineStr"/>
@@ -15367,7 +15367,7 @@
       </c>
       <c r="R142" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S142" t="inlineStr"/>
@@ -15471,7 +15471,7 @@
       </c>
       <c r="R143" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>f32cdab</t>
         </is>
       </c>
       <c r="S143" t="inlineStr"/>
@@ -15579,7 +15579,7 @@
       </c>
       <c r="R144" t="inlineStr">
         <is>
-          <t>BIT 0</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S144" t="inlineStr"/>
@@ -15687,7 +15687,7 @@
       </c>
       <c r="R145" t="inlineStr">
         <is>
-          <t>BIT 1</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S145" t="inlineStr"/>
@@ -15795,7 +15795,7 @@
       </c>
       <c r="R146" t="inlineStr">
         <is>
-          <t>BIT 2</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S146" t="inlineStr"/>
@@ -15903,7 +15903,7 @@
       </c>
       <c r="R147" t="inlineStr">
         <is>
-          <t>BIT 3</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S147" t="inlineStr"/>
@@ -16011,7 +16011,7 @@
       </c>
       <c r="R148" t="inlineStr">
         <is>
-          <t>BIT 4</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S148" t="inlineStr"/>
@@ -16119,7 +16119,7 @@
       </c>
       <c r="R149" t="inlineStr">
         <is>
-          <t>BIT 5</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S149" t="inlineStr"/>
@@ -16227,7 +16227,7 @@
       </c>
       <c r="R150" t="inlineStr">
         <is>
-          <t>BIT 6</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S150" t="inlineStr"/>
@@ -16335,7 +16335,7 @@
       </c>
       <c r="R151" t="inlineStr">
         <is>
-          <t>BIT 7</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S151" t="inlineStr"/>
@@ -16443,7 +16443,7 @@
       </c>
       <c r="R152" t="inlineStr">
         <is>
-          <t>BIT 8</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S152" t="inlineStr"/>
@@ -16551,7 +16551,7 @@
       </c>
       <c r="R153" t="inlineStr">
         <is>
-          <t>BIT 9</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S153" t="inlineStr"/>
@@ -16659,7 +16659,7 @@
       </c>
       <c r="R154" t="inlineStr">
         <is>
-          <t>BIT 10</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S154" t="inlineStr"/>
@@ -16767,7 +16767,7 @@
       </c>
       <c r="R155" t="inlineStr">
         <is>
-          <t>BIT 11</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S155" t="inlineStr"/>
@@ -16875,7 +16875,7 @@
       </c>
       <c r="R156" t="inlineStr">
         <is>
-          <t>BIT 12</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S156" t="inlineStr"/>
@@ -16983,7 +16983,7 @@
       </c>
       <c r="R157" t="inlineStr">
         <is>
-          <t>BIT 13</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S157" t="inlineStr"/>
@@ -17091,7 +17091,7 @@
       </c>
       <c r="R158" t="inlineStr">
         <is>
-          <t>BIT 14</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S158" t="inlineStr"/>
@@ -17199,7 +17199,7 @@
       </c>
       <c r="R159" t="inlineStr">
         <is>
-          <t>BIT 15</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S159" t="inlineStr"/>
@@ -17307,7 +17307,7 @@
       </c>
       <c r="R160" t="inlineStr">
         <is>
-          <t>BIT 16</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S160" t="inlineStr"/>
@@ -17415,7 +17415,7 @@
       </c>
       <c r="R161" t="inlineStr">
         <is>
-          <t>BIT 17</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S161" t="inlineStr"/>
@@ -17523,7 +17523,7 @@
       </c>
       <c r="R162" t="inlineStr">
         <is>
-          <t>BIT 18</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S162" t="inlineStr"/>
@@ -17631,7 +17631,7 @@
       </c>
       <c r="R163" t="inlineStr">
         <is>
-          <t>BIT 19</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S163" t="inlineStr"/>
@@ -17739,7 +17739,7 @@
       </c>
       <c r="R164" t="inlineStr">
         <is>
-          <t>BIT 20</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S164" t="inlineStr"/>
@@ -17847,7 +17847,7 @@
       </c>
       <c r="R165" t="inlineStr">
         <is>
-          <t>BIT 21</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S165" t="inlineStr"/>
@@ -17955,7 +17955,7 @@
       </c>
       <c r="R166" t="inlineStr">
         <is>
-          <t>BIT 22</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S166" t="inlineStr"/>
@@ -18063,7 +18063,7 @@
       </c>
       <c r="R167" t="inlineStr">
         <is>
-          <t>BIT 23</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S167" t="inlineStr"/>
@@ -18171,7 +18171,7 @@
       </c>
       <c r="R168" t="inlineStr">
         <is>
-          <t>BIT 24</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S168" t="inlineStr"/>
@@ -18279,7 +18279,7 @@
       </c>
       <c r="R169" t="inlineStr">
         <is>
-          <t>BIT 25</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S169" t="inlineStr"/>
@@ -18387,7 +18387,7 @@
       </c>
       <c r="R170" t="inlineStr">
         <is>
-          <t>BIT 26</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S170" t="inlineStr"/>
@@ -18495,7 +18495,7 @@
       </c>
       <c r="R171" t="inlineStr">
         <is>
-          <t>BIT 27</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S171" t="inlineStr"/>
@@ -18603,7 +18603,7 @@
       </c>
       <c r="R172" t="inlineStr">
         <is>
-          <t>BIT 28</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S172" t="inlineStr"/>
@@ -18711,7 +18711,7 @@
       </c>
       <c r="R173" t="inlineStr">
         <is>
-          <t>BIT 29</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S173" t="inlineStr"/>
@@ -18819,7 +18819,7 @@
       </c>
       <c r="R174" t="inlineStr">
         <is>
-          <t>BIT 30</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S174" t="inlineStr"/>
@@ -18927,7 +18927,7 @@
       </c>
       <c r="R175" t="inlineStr">
         <is>
-          <t>BIT 31</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S175" t="inlineStr"/>
@@ -19035,7 +19035,7 @@
       </c>
       <c r="R176" t="inlineStr">
         <is>
-          <t>BIT 0</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S176" t="inlineStr"/>
@@ -19143,7 +19143,7 @@
       </c>
       <c r="R177" t="inlineStr">
         <is>
-          <t>BIT 1</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S177" t="inlineStr"/>
@@ -19251,7 +19251,7 @@
       </c>
       <c r="R178" t="inlineStr">
         <is>
-          <t>BIT 2</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S178" t="inlineStr"/>
@@ -19359,7 +19359,7 @@
       </c>
       <c r="R179" t="inlineStr">
         <is>
-          <t>BIT 3</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S179" t="inlineStr"/>
@@ -19467,7 +19467,7 @@
       </c>
       <c r="R180" t="inlineStr">
         <is>
-          <t>BIT 4</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S180" t="inlineStr"/>
@@ -19575,7 +19575,7 @@
       </c>
       <c r="R181" t="inlineStr">
         <is>
-          <t>BIT 5</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S181" t="inlineStr"/>
@@ -19679,7 +19679,7 @@
       </c>
       <c r="R182" t="inlineStr">
         <is>
-          <t>BIT 6</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S182" t="inlineStr"/>
@@ -19783,7 +19783,7 @@
       </c>
       <c r="R183" t="inlineStr">
         <is>
-          <t>BIT 7</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S183" t="inlineStr"/>
@@ -19887,7 +19887,7 @@
       </c>
       <c r="R184" t="inlineStr">
         <is>
-          <t>BIT 8</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S184" t="inlineStr"/>
@@ -19991,7 +19991,7 @@
       </c>
       <c r="R185" t="inlineStr">
         <is>
-          <t>BIT 9</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S185" t="inlineStr"/>
@@ -20095,7 +20095,7 @@
       </c>
       <c r="R186" t="inlineStr">
         <is>
-          <t>BIT 10</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S186" t="inlineStr"/>
@@ -20199,7 +20199,7 @@
       </c>
       <c r="R187" t="inlineStr">
         <is>
-          <t>BIT 11</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S187" t="inlineStr"/>
@@ -20303,7 +20303,7 @@
       </c>
       <c r="R188" t="inlineStr">
         <is>
-          <t>BIT 12</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S188" t="inlineStr"/>
@@ -20407,7 +20407,7 @@
       </c>
       <c r="R189" t="inlineStr">
         <is>
-          <t>BIT 13</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S189" t="inlineStr"/>
@@ -20511,7 +20511,7 @@
       </c>
       <c r="R190" t="inlineStr">
         <is>
-          <t>BIT 14</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S190" t="inlineStr"/>
@@ -20615,7 +20615,7 @@
       </c>
       <c r="R191" t="inlineStr">
         <is>
-          <t>BIT 15</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S191" t="inlineStr"/>
@@ -20719,7 +20719,7 @@
       </c>
       <c r="R192" t="inlineStr">
         <is>
-          <t>BIT 16</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S192" t="inlineStr"/>
@@ -20823,7 +20823,7 @@
       </c>
       <c r="R193" t="inlineStr">
         <is>
-          <t>BIT 17</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S193" t="inlineStr"/>
@@ -20927,7 +20927,7 @@
       </c>
       <c r="R194" t="inlineStr">
         <is>
-          <t>BIT 18</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S194" t="inlineStr"/>
@@ -21031,7 +21031,7 @@
       </c>
       <c r="R195" t="inlineStr">
         <is>
-          <t>BIT 19</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S195" t="inlineStr"/>
@@ -21135,7 +21135,7 @@
       </c>
       <c r="R196" t="inlineStr">
         <is>
-          <t>BIT 20</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S196" t="inlineStr"/>
@@ -21239,7 +21239,7 @@
       </c>
       <c r="R197" t="inlineStr">
         <is>
-          <t>BIT 21</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S197" t="inlineStr"/>
@@ -21343,7 +21343,7 @@
       </c>
       <c r="R198" t="inlineStr">
         <is>
-          <t>BIT 22</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S198" t="inlineStr"/>
@@ -21447,7 +21447,7 @@
       </c>
       <c r="R199" t="inlineStr">
         <is>
-          <t>BIT 23</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S199" t="inlineStr"/>
@@ -21551,7 +21551,7 @@
       </c>
       <c r="R200" t="inlineStr">
         <is>
-          <t>BIT 24</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S200" t="inlineStr"/>
@@ -21655,7 +21655,7 @@
       </c>
       <c r="R201" t="inlineStr">
         <is>
-          <t>BIT 25</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S201" t="inlineStr"/>
@@ -21759,7 +21759,7 @@
       </c>
       <c r="R202" t="inlineStr">
         <is>
-          <t>BIT 26</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S202" t="inlineStr"/>
@@ -21863,7 +21863,7 @@
       </c>
       <c r="R203" t="inlineStr">
         <is>
-          <t>BIT 27</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S203" t="inlineStr"/>
@@ -21967,7 +21967,7 @@
       </c>
       <c r="R204" t="inlineStr">
         <is>
-          <t>BIT 28</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S204" t="inlineStr"/>
@@ -22071,7 +22071,7 @@
       </c>
       <c r="R205" t="inlineStr">
         <is>
-          <t>BIT 29</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S205" t="inlineStr"/>
@@ -22175,7 +22175,7 @@
       </c>
       <c r="R206" t="inlineStr">
         <is>
-          <t>BIT 30</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S206" t="inlineStr"/>
@@ -22279,7 +22279,7 @@
       </c>
       <c r="R207" t="inlineStr">
         <is>
-          <t>BIT 31</t>
+          <t>1bit</t>
         </is>
       </c>
       <c r="S207" t="inlineStr"/>

</xml_diff>